<commit_message>
CAMPY updated to classes
instances from EFSA
</commit_message>
<xml_diff>
--- a/docs/campy_efsa.xlsx
+++ b/docs/campy_efsa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernanda.dorea\Documents\GitHub\HSO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE013F2-7CB8-4B0E-8BA3-48652AF27883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACA3131-F8E2-47AB-855F-CBA9EA6654C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13707" xr2:uid="{BC9F9AC6-E6B5-4E26-8DC4-44951FDC5054}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
   <si>
     <t>URI</t>
   </si>
@@ -77,33 +77,12 @@
     <t>RF-00000066-MCG</t>
   </si>
   <si>
-    <t>Campylobacter, unspecified sp.</t>
-  </si>
-  <si>
     <t>RF-00000044-MCG</t>
   </si>
   <si>
-    <t>thermotolerant Campylobacter, unspecified</t>
-  </si>
-  <si>
     <t>RF-00000052-MCG</t>
   </si>
   <si>
-    <t>HasRelatedSynonym</t>
-  </si>
-  <si>
-    <t>Campylobacter jejuni jejuni</t>
-  </si>
-  <si>
-    <t>hasExactSynonym</t>
-  </si>
-  <si>
-    <t>isSubSpeciesOf</t>
-  </si>
-  <si>
-    <t>Campylobacter spp</t>
-  </si>
-  <si>
     <t>https://w3id.org/hso#PARAM_RF-00000050-MCG</t>
   </si>
   <si>
@@ -135,6 +114,222 @@
   </si>
   <si>
     <t>URI2</t>
+  </si>
+  <si>
+    <t>Campylobacter coli</t>
+  </si>
+  <si>
+    <t>RF-00000054-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter curvus</t>
+  </si>
+  <si>
+    <t>RF-00000049-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter fetus</t>
+  </si>
+  <si>
+    <t>RF-00000055-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter fetus subsp. fetus</t>
+  </si>
+  <si>
+    <t>RF-00000056-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter fetus subsp. venerealis</t>
+  </si>
+  <si>
+    <t>RF-00000057-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter gracilis</t>
+  </si>
+  <si>
+    <t>RF-00000053-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter hominis</t>
+  </si>
+  <si>
+    <t>RF-00000051-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter hyointestinalis</t>
+  </si>
+  <si>
+    <t>RF-00000058-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter hyointestinalis subsp. hyointestinalis</t>
+  </si>
+  <si>
+    <t>RF-00000060-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter hyointestinalis subsp. lawsonii</t>
+  </si>
+  <si>
+    <t>RF-00000059-MCG</t>
+  </si>
+  <si>
+    <t>RF-00000061-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter lari</t>
+  </si>
+  <si>
+    <t>RF-00000048-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter mucosalis</t>
+  </si>
+  <si>
+    <t>RF-00000047-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter rectus</t>
+  </si>
+  <si>
+    <t>RF-00000045-MCG</t>
+  </si>
+  <si>
+    <t>RF-00000064-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter sputorum biovar sputorum</t>
+  </si>
+  <si>
+    <t>RF-00000067-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter sputorum subsp. bubulus</t>
+  </si>
+  <si>
+    <t>RF-00000065-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter upsaliensis</t>
+  </si>
+  <si>
+    <t>RF-00000043-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000054-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000049-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000055-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000056-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000057-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000053-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000051-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000058-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000060-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000059-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000061-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000048-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000047-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000045-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000064-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000067-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000065-MCG</t>
+  </si>
+  <si>
+    <t>PARAM_RF-00000043-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000054-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000049-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000055-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000056-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000057-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000053-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000051-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000058-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000060-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000059-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000061-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000048-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000047-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000045-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000064-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000067-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000065-MCG</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hso#PARAM_RF-00000043-MCG</t>
+  </si>
+  <si>
+    <t>Campylobacter unspecified sp.</t>
+  </si>
+  <si>
+    <t>thermotolerant Campylobacter unspecified</t>
   </si>
 </sst>
 </file>
@@ -179,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -187,7 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -504,21 +698,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A4E8FD-7C3F-40B9-AE91-C71BF98B3EC8}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.875" customWidth="1"/>
     <col min="2" max="2" width="30.625" customWidth="1"/>
-    <col min="10" max="10" width="28.875" customWidth="1"/>
-    <col min="11" max="11" width="53.875" customWidth="1"/>
+    <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,27 +728,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -566,16 +744,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -586,19 +761,13 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -609,59 +778,442 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
+      <c r="F29" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location="PARAM_RF-00000050-MCG" display="https://w3id.org/hso#PARAM_RF-00000050-MCG" xr:uid="{292AF015-6381-4F95-9D57-228EBECC1EAC}"/>
-    <hyperlink ref="K2" r:id="rId2" location="PARAM_RF-00000050-MCG" xr:uid="{B45638CC-FEE3-43B4-89A2-FEE5E44D04CF}"/>
+    <hyperlink ref="F2" r:id="rId2" location="PARAM_RF-00000050-MCG" xr:uid="{B45638CC-FEE3-43B4-89A2-FEE5E44D04CF}"/>
+    <hyperlink ref="F6" r:id="rId3" location="PARAM_RF-00000052-MCG" xr:uid="{68D3FADA-DD59-4E8E-A832-919D41998EBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>